<commit_message>
New and updated examples traffic
Added examples for traffic incidents, updated specification for traffic observations according to changes in ontology.
</commit_message>
<xml_diff>
--- a/examples/traffic/InputTraffic.xlsx
+++ b/examples/traffic/InputTraffic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ednaruckhaus/Documents/GitHub/Mapeathor/examples/traffic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8E4477C-2DE8-D947-B360-A6C791BC59C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61DEC2D9-1DC3-3942-BB07-2C335517E3A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3500" yWindow="460" windowWidth="19520" windowHeight="15760" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10520" yWindow="2900" windowWidth="19520" windowHeight="15760" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prefixes" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="PredicateObjectMaps" sheetId="4" r:id="rId4"/>
     <sheet name="Functions" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="104">
   <si>
     <t>Prefix</t>
   </si>
@@ -133,12 +133,6 @@
     <t>boolean</t>
   </si>
   <si>
-    <t>geosparql:lat</t>
-  </si>
-  <si>
-    <t>geosparql:long</t>
-  </si>
-  <si>
     <t>double</t>
   </si>
   <si>
@@ -202,9 +196,6 @@
     <t>estraf:urbano</t>
   </si>
   <si>
-    <t>{tipo}</t>
-  </si>
-  <si>
     <t>estraf:enServicio</t>
   </si>
   <si>
@@ -229,9 +220,6 @@
     <t>examples/Traffic/estaciones.csv</t>
   </si>
   <si>
-    <t>examples/Traffic/observaciones.xml</t>
-  </si>
-  <si>
     <t>sosa:hasSimpleResult</t>
   </si>
   <si>
@@ -262,9 +250,6 @@
     <t>http://vocab.ciudadesabiertas.es/recurso/transporte/trafico/</t>
   </si>
   <si>
-    <t>recurso-trafico:punto/{p}-{id}</t>
-  </si>
-  <si>
     <t>{longitud}</t>
   </si>
   <si>
@@ -295,15 +280,6 @@
     <t>sosa:madeBySensor</t>
   </si>
   <si>
-    <t>http://vocab.ciudadesabiertas.es/recurso/transporte/trafico/observacion/{fecha_hora}-{idelem}-carga</t>
-  </si>
-  <si>
-    <t>http://vocab.ciudadesabiertas.es/recurso/transporte/trafico/observacion/{fecha_hora}-{idelem}-intensidad</t>
-  </si>
-  <si>
-    <t>http://vocab.ciudadesabiertas.es/recurso/transporte/trafico/observacion/{fecha_hora}-{idelem}-ocupacion</t>
-  </si>
-  <si>
     <t>idObservacionCarga</t>
   </si>
   <si>
@@ -323,6 +299,48 @@
   </si>
   <si>
     <t>{ocupacion}</t>
+  </si>
+  <si>
+    <t>idPunto</t>
+  </si>
+  <si>
+    <t>http://vocab.ciudadesabiertas.es/recurso/transporte/trafico/punto/p-{id}</t>
+  </si>
+  <si>
+    <t>recurso-trafico:punto/p-{id}</t>
+  </si>
+  <si>
+    <t>examples/Traffic/observaciones.csv</t>
+  </si>
+  <si>
+    <t>http://vocab.ciudadesabiertas.es/recurso/transporte/trafico/observacion/{fechaid}-{idelem}-carga</t>
+  </si>
+  <si>
+    <t>http://vocab.ciudadesabiertas.es/recurso/transporte/trafico/observacion/{fechaid}-{idelem}-intensidad</t>
+  </si>
+  <si>
+    <t>http://vocab.ciudadesabiertas.es/recurso/transporte/trafico/observacion/{fechaid}-{idelem}-ocupacion</t>
+  </si>
+  <si>
+    <t>sf</t>
+  </si>
+  <si>
+    <t>http://www.opengis.net/ont/sf#</t>
+  </si>
+  <si>
+    <t>gf:Point</t>
+  </si>
+  <si>
+    <t>geo:lat</t>
+  </si>
+  <si>
+    <t>geo:long</t>
+  </si>
+  <si>
+    <t>estraf:validado</t>
+  </si>
+  <si>
+    <t>false</t>
   </si>
 </sst>
 </file>
@@ -707,10 +725,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -733,7 +751,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -741,7 +759,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -749,7 +767,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -757,7 +775,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -765,7 +783,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -773,7 +791,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -781,7 +799,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -789,7 +807,7 @@
         <v>28</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -797,7 +815,7 @@
         <v>29</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -805,7 +823,7 @@
         <v>30</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -813,7 +831,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -821,31 +839,39 @@
         <v>31</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>76</v>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>97</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -856,10 +882,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -881,18 +907,18 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s">
         <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
         <v>14</v>
@@ -903,18 +929,18 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B5" t="s">
         <v>14</v>
@@ -925,18 +951,18 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="B6" t="s">
         <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>66</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="B7" t="s">
         <v>14</v>
@@ -947,23 +973,45 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>66</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
       </c>
       <c r="C9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
         <v>15</v>
       </c>
     </row>
@@ -975,10 +1023,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1001,101 +1049,112 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>49</v>
-      </c>
-      <c r="B2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>49</v>
-      </c>
-      <c r="B3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C4" s="7" t="s">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>91</v>
-      </c>
-      <c r="B5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>92</v>
-      </c>
-      <c r="B6" t="s">
-        <v>53</v>
-      </c>
       <c r="C6" s="7" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="B7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B8" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="B9" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="B10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>90</v>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1106,10 +1165,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1152,13 +1211,13 @@
         <v>26</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C2" t="s">
         <v>24</v>
       </c>
       <c r="G2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1166,35 +1225,35 @@
         <v>27</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C3" t="s">
         <v>24</v>
       </c>
       <c r="G3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>56</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>57</v>
       </c>
       <c r="C4" t="s">
         <v>33</v>
       </c>
       <c r="G4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C5" t="s">
         <v>33</v>
@@ -1209,254 +1268,262 @@
         <v>32</v>
       </c>
       <c r="G5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C7" t="s">
         <v>23</v>
       </c>
       <c r="G7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B8" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="C8" t="s">
         <v>23</v>
       </c>
       <c r="G8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" t="s">
         <v>34</v>
       </c>
-      <c r="B9" t="s">
-        <v>78</v>
-      </c>
-      <c r="C9" t="s">
-        <v>36</v>
-      </c>
       <c r="G9" t="s">
-        <v>49</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>101</v>
       </c>
       <c r="B10" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G10" t="s">
-        <v>49</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B11" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C11" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="G11" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B12" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C12" t="s">
         <v>23</v>
       </c>
       <c r="G12" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E13" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="F13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G13" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B14" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="C14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G14" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B15" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C15" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="G15" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>83</v>
-      </c>
-      <c r="B16" t="s">
-        <v>85</v>
-      </c>
-      <c r="C16" t="s">
-        <v>23</v>
-      </c>
-      <c r="G16" t="s">
-        <v>92</v>
+        <v>102</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>87</v>
-      </c>
-      <c r="D17" t="s">
-        <v>49</v>
-      </c>
-      <c r="E17" t="s">
-        <v>96</v>
-      </c>
-      <c r="F17" t="s">
-        <v>54</v>
+        <v>78</v>
+      </c>
+      <c r="B17" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" t="s">
+        <v>23</v>
       </c>
       <c r="G17" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>67</v>
-      </c>
-      <c r="B18" t="s">
-        <v>95</v>
-      </c>
-      <c r="C18" t="s">
-        <v>36</v>
+        <v>82</v>
+      </c>
+      <c r="D18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" t="s">
+        <v>88</v>
+      </c>
+      <c r="F18" t="s">
+        <v>52</v>
       </c>
       <c r="G18" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="B19" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="C19" t="s">
-        <v>82</v>
+        <v>34</v>
       </c>
       <c r="G19" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B20" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="C20" t="s">
-        <v>23</v>
+        <v>77</v>
       </c>
       <c r="G20" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>87</v>
-      </c>
-      <c r="D21" t="s">
-        <v>49</v>
-      </c>
-      <c r="E21" t="s">
-        <v>96</v>
-      </c>
-      <c r="F21" t="s">
-        <v>54</v>
+        <v>78</v>
+      </c>
+      <c r="B21" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" t="s">
+        <v>23</v>
       </c>
       <c r="G21" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>67</v>
-      </c>
-      <c r="B22" t="s">
-        <v>97</v>
-      </c>
-      <c r="C22" t="s">
-        <v>36</v>
+        <v>82</v>
+      </c>
+      <c r="D22" t="s">
+        <v>47</v>
+      </c>
+      <c r="E22" t="s">
+        <v>88</v>
+      </c>
+      <c r="F22" t="s">
+        <v>52</v>
       </c>
       <c r="G22" t="s">
-        <v>93</v>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" t="s">
+        <v>89</v>
+      </c>
+      <c r="C23" t="s">
+        <v>34</v>
+      </c>
+      <c r="G23" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mappings for case study vocabulary Urban Public Bus (Ciudades Abiertas)
Mappings were generated for data on urban buses in Madrid following the Public Bus ontology in Ciudades Abiertas which in turn is aligned with the Transmodel standard model. Data were generated for lines, some routes and all of the stops.
</commit_message>
<xml_diff>
--- a/examples/traffic/InputTraffic.xlsx
+++ b/examples/traffic/InputTraffic.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ednaruckhaus/Documents/GitHub/Mapeathor/examples/traffic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A909F5DB-E083-1749-8EE5-DA745A0ED8EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A682665B-64B2-0A4E-9986-643EBD874C23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3960" yWindow="1300" windowWidth="19520" windowHeight="15760" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3960" yWindow="1300" windowWidth="19520" windowHeight="15760" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prefixes" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="PredicateObjectMaps" sheetId="4" r:id="rId4"/>
     <sheet name="Functions" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -336,9 +336,6 @@
     <t>http://www.opengis.net/ont/sf#</t>
   </si>
   <si>
-    <t>gf:Point</t>
-  </si>
-  <si>
     <t>geo:lat</t>
   </si>
   <si>
@@ -349,6 +346,9 @@
   </si>
   <si>
     <t>false</t>
+  </si>
+  <si>
+    <t>sf:Point</t>
   </si>
 </sst>
 </file>
@@ -1048,7 +1048,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1107,7 +1107,7 @@
         <v>90</v>
       </c>
       <c r="B5" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>91</v>
@@ -1189,8 +1189,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView topLeftCell="A3" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1337,7 +1337,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B9" t="s">
         <v>73</v>
@@ -1351,7 +1351,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B10" t="s">
         <v>74</v>
@@ -1438,10 +1438,10 @@
     </row>
     <row r="16" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>101</v>
+      </c>
+      <c r="B16" s="8" t="s">
         <v>102</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -1558,7 +1558,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>